<commit_message>
Updated for work with advanced circuits
</commit_message>
<xml_diff>
--- a/Project Outputs for BMSSlaveBoard/BMSSlaveBoard-BOM.xlsx
+++ b/Project Outputs for BMSSlaveBoard/BMSSlaveBoard-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pilot\Documents\FSAE\BMS\f29bms-slaveboard\Project Outputs for BMSSlaveBoard\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spb35\Desktop\Projects\F28\f29bms-slaveboard\Project Outputs for BMSSlaveBoard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE716EB-9227-44A1-8C14-A4593137A5E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A5B52C-780A-41B4-8CE4-E5CE104AB77B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27450" yWindow="15" windowWidth="24975" windowHeight="13785" xr2:uid="{27CA359D-1E37-4901-A651-D5D80B096E5A}"/>
+    <workbookView xWindow="30" yWindow="600" windowWidth="28770" windowHeight="15600" xr2:uid="{27CA359D-1E37-4901-A651-D5D80B096E5A}"/>
   </bookViews>
   <sheets>
     <sheet name="BMSSlaveBoard-BOM" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
   <si>
     <t>Comment</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>LibRef</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>FP-CL21-IPC_A</t>
   </si>
   <si>
-    <t>CMP-13271-003077-1</t>
-  </si>
-  <si>
     <t>CL10B104KC8NNNC</t>
   </si>
   <si>
@@ -84,9 +78,6 @@
     <t>FP-CL10-IPC_A</t>
   </si>
   <si>
-    <t>CMP-13271-004036-1</t>
-  </si>
-  <si>
     <t>CC0603KRX7R9BB105</t>
   </si>
   <si>
@@ -99,9 +90,6 @@
     <t>FP-CC0603-DB-MFG</t>
   </si>
   <si>
-    <t>CMP-03422-000761-2</t>
-  </si>
-  <si>
     <t>Green</t>
   </si>
   <si>
@@ -114,9 +102,6 @@
     <t>LED, TH</t>
   </si>
   <si>
-    <t>TLHG6400CS12Z</t>
-  </si>
-  <si>
     <t>3404.0112.11</t>
   </si>
   <si>
@@ -141,9 +126,6 @@
     <t>0856-0</t>
   </si>
   <si>
-    <t>0856-0-15-20-82-14-11-0</t>
-  </si>
-  <si>
     <t>1726480103</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t>FP-DLW43-0_2-t2_6-e0_6-MFG</t>
   </si>
   <si>
-    <t>CMP-06045-000059-1</t>
-  </si>
-  <si>
     <t>NDS332P</t>
   </si>
   <si>
@@ -207,9 +186,6 @@
     <t>ONSC-SOT-223-4-318E-04_V</t>
   </si>
   <si>
-    <t>CMP-1048-00450-1</t>
-  </si>
-  <si>
     <t>RK73B2ATTD101J</t>
   </si>
   <si>
@@ -222,9 +198,6 @@
     <t>RESC2013X60X30NL20T20</t>
   </si>
   <si>
-    <t>CMP-2001-04655-1</t>
-  </si>
-  <si>
     <t>RC0805JR-073K3L</t>
   </si>
   <si>
@@ -237,9 +210,6 @@
     <t>RESC0805(2012)_M</t>
   </si>
   <si>
-    <t>CMP-1013-00086-1</t>
-  </si>
-  <si>
     <t>16R 2W</t>
   </si>
   <si>
@@ -252,9 +222,6 @@
     <t>TH16R</t>
   </si>
   <si>
-    <t>NKN200FR-73-16R</t>
-  </si>
-  <si>
     <t>AC0603FR-07180RL</t>
   </si>
   <si>
@@ -291,9 +258,6 @@
     <t>RESC3225X70X50LL20T20</t>
   </si>
   <si>
-    <t>CMP-2005-03479-1</t>
-  </si>
-  <si>
     <t>ERJ-PB3B1002V</t>
   </si>
   <si>
@@ -315,9 +279,6 @@
     <t>RESC1206(3216)_N</t>
   </si>
   <si>
-    <t>CMP-1014-00373-1</t>
-  </si>
-  <si>
     <t>AC1206FR-0749R9L</t>
   </si>
   <si>
@@ -330,9 +291,6 @@
     <t>FP-AC1206-MFG</t>
   </si>
   <si>
-    <t>CMP-03412-027409-1</t>
-  </si>
-  <si>
     <t>RC0603FR-071K21L</t>
   </si>
   <si>
@@ -345,18 +303,12 @@
     <t>RESC1608X55X25LL10T15</t>
   </si>
   <si>
-    <t>CMP-2000-03933-1</t>
-  </si>
-  <si>
     <t>RC0603FR-07806RL</t>
   </si>
   <si>
     <t>R22, R30</t>
   </si>
   <si>
-    <t>CMP-2000-04142-1</t>
-  </si>
-  <si>
     <t>PE-68386NLT</t>
   </si>
   <si>
@@ -379,9 +331,6 @@
   </si>
   <si>
     <t>LT-G-48_M</t>
-  </si>
-  <si>
-    <t>CMP-0471-00242-1</t>
   </si>
 </sst>
 </file>
@@ -423,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -446,11 +395,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
@@ -460,6 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -777,15 +738,16 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -804,487 +766,413 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="6">
+      <c r="E2" s="6">
         <v>24</v>
       </c>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="6">
+      <c r="E3" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6">
+      <c r="E4" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="6">
+        <v>20</v>
+      </c>
+      <c r="E5" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="6">
+        <v>24</v>
+      </c>
+      <c r="E6" s="6">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F7" s="6">
+        <v>28</v>
+      </c>
+      <c r="E7" s="6">
         <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="6">
+        <v>32</v>
+      </c>
+      <c r="E8" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="6">
+        <v>36</v>
+      </c>
+      <c r="E9" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="6">
+        <v>40</v>
+      </c>
+      <c r="E10" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="6">
+        <v>44</v>
+      </c>
+      <c r="E11" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" s="6">
+        <v>48</v>
+      </c>
+      <c r="E12" s="6">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="8">
+        <v>52</v>
+      </c>
+      <c r="E13" s="8">
         <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="E14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="6">
+        <v>56</v>
+      </c>
+      <c r="E14" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="F15" s="6">
+        <v>60</v>
+      </c>
+      <c r="E15" s="6">
         <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="E18" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="C19" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="F16" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="D19" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B20" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C20" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D20" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E17" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="6">
+      <c r="E20" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B21" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E21" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
+      <c r="B22" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="D22" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="E19" s="7" t="s">
+      <c r="E22" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F19" s="8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="B20" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D23" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="C24" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F20" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="E24" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="C25" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="D25" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F21" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="F22" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="F23" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="F24" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="F25" s="1">
+      <c r="E25" s="1">
         <v>2</v>
       </c>
     </row>

</xml_diff>